<commit_message>
Added more data - new boards added recently
</commit_message>
<xml_diff>
--- a/src/DbScript/BoardsData.xlsx
+++ b/src/DbScript/BoardsData.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="BoardsData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="621">
   <si>
     <t>administration</t>
   </si>
@@ -1681,6 +1681,210 @@
   </si>
   <si>
     <t>Keyboard training</t>
+  </si>
+  <si>
+    <t>color_mix</t>
+  </si>
+  <si>
+    <t>color_mix.svg</t>
+  </si>
+  <si>
+    <t>Mixing color of paint</t>
+  </si>
+  <si>
+    <t>To understand color mixing.</t>
+  </si>
+  <si>
+    <t>Mix the primary colors to match to the given color</t>
+  </si>
+  <si>
+    <t>color_mix_light</t>
+  </si>
+  <si>
+    <t>color_mix_light.svg</t>
+  </si>
+  <si>
+    <t>Mixing colors of light</t>
+  </si>
+  <si>
+    <t>Understanding mixing of colors of light.</t>
+  </si>
+  <si>
+    <t>Mix the primary colors to match to the given color.</t>
+  </si>
+  <si>
+    <t>explore_farm_animals</t>
+  </si>
+  <si>
+    <t>explore_farm_animals.svg</t>
+  </si>
+  <si>
+    <t>Explore Farm Animals</t>
+  </si>
+  <si>
+    <t>Learn about farm animals, what sounds they make, and interesting facts.</t>
+  </si>
+  <si>
+    <t>Learn to associate animal sounds with the animal name and what the animal looks like.</t>
+  </si>
+  <si>
+    <t>explore_world_animals</t>
+  </si>
+  <si>
+    <t>explore_world_animals.svg</t>
+  </si>
+  <si>
+    <t>Explore World Animals</t>
+  </si>
+  <si>
+    <t>Learn about world animals, interesting facts and their location on a map.</t>
+  </si>
+  <si>
+    <t>explore_world_music</t>
+  </si>
+  <si>
+    <t>explore_world_music.svg</t>
+  </si>
+  <si>
+    <t>Explore World Music</t>
+  </si>
+  <si>
+    <t>Learn about the music of the world.</t>
+  </si>
+  <si>
+    <t>Develop a better understanding of the variety of music present in the world</t>
+  </si>
+  <si>
+    <t>intro_gravity</t>
+  </si>
+  <si>
+    <t>intro_gravity.svg</t>
+  </si>
+  <si>
+    <t>Intro gravity</t>
+  </si>
+  <si>
+    <t>Introduction to the concept of gravity</t>
+  </si>
+  <si>
+    <t>Maintain the spaceship in the middle without crashing into the planets or the asteroids</t>
+  </si>
+  <si>
+    <t>land_safe</t>
+  </si>
+  <si>
+    <t>land_safe.svg</t>
+  </si>
+  <si>
+    <t>Land Safe</t>
+  </si>
+  <si>
+    <t>Understanding acceleration due to gravity.</t>
+  </si>
+  <si>
+    <t>Pilot the spaceship towards the green landing area.</t>
+  </si>
+  <si>
+    <t>mining</t>
+  </si>
+  <si>
+    <t>mining.svg</t>
+  </si>
+  <si>
+    <t>Mining for gold</t>
+  </si>
+  <si>
+    <t>Use the mousewheel to approach the rockwall an look for gold nuggets.</t>
+  </si>
+  <si>
+    <t>You should be familiar with moving the mouse and clicking.</t>
+  </si>
+  <si>
+    <t>Learn to use the mousewheel to zoom in and out.</t>
+  </si>
+  <si>
+    <t>note_names</t>
+  </si>
+  <si>
+    <t>note_names.svg</t>
+  </si>
+  <si>
+    <t>Name that Note!</t>
+  </si>
+  <si>
+    <t>Learn the names of the notes, in bass and treble clef, with the help of sounds and colors</t>
+  </si>
+  <si>
+    <t>To develop a good understanding of note position and naming convention. To prepare for the piano player and composition activity</t>
+  </si>
+  <si>
+    <t>piano_composition</t>
+  </si>
+  <si>
+    <t>piano_composition.svg</t>
+  </si>
+  <si>
+    <t>Piano Composition</t>
+  </si>
+  <si>
+    <t>An activity to learn how the piano keyboard works, how notes are written on a musical staff and explore music composition by loading and saving your work.</t>
+  </si>
+  <si>
+    <t>Familiarity with note naming conventions, note-names activity useful to learn this notation.</t>
+  </si>
+  <si>
+    <t>Develop an understanding of music composition, and increase interest in making music with a piano keyboard. This activity covers many fundamental aspects of music, but there is much more to explore about music composition. If you enjoy this activity but want a more advanced tool, try downloading MuseScore (http://musescore.org/en/download), an open source music notation tool.</t>
+  </si>
+  <si>
+    <t>place_your_satellite</t>
+  </si>
+  <si>
+    <t>place_your_satellite.svg</t>
+  </si>
+  <si>
+    <t>Place your satellite</t>
+  </si>
+  <si>
+    <t>Understanding effect of mass and distance on orbital velocity.</t>
+  </si>
+  <si>
+    <t>Make sure the satellite does not crash or fly away</t>
+  </si>
+  <si>
+    <t>play_piano</t>
+  </si>
+  <si>
+    <t>play_piano.svg</t>
+  </si>
+  <si>
+    <t>Play Piano!</t>
+  </si>
+  <si>
+    <t>Learn to play melodies on the piano keyboard!</t>
+  </si>
+  <si>
+    <t>Knowledge of musical notation and musical staff. Play the activity named 'Piano Composition' first.</t>
+  </si>
+  <si>
+    <t>Understand how the piano keyboard can play music as written on the musical staff.</t>
+  </si>
+  <si>
+    <t>play_rhythm</t>
+  </si>
+  <si>
+    <t>play_rhythm.svg</t>
+  </si>
+  <si>
+    <t>Play Rhythm</t>
+  </si>
+  <si>
+    <t>Learn to listen to, read, and play musical rhythms.</t>
+  </si>
+  <si>
+    <t>Simple understanding of musical rhythm and beat.</t>
+  </si>
+  <si>
+    <t>Learn to beat rhythms precisely and accurately based on what you see and hear.</t>
   </si>
 </sst>
 </file>
@@ -2512,10 +2716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H153"/>
+  <dimension ref="A1:Q168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A153"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,7 +2728,7 @@
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="225" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4147,7 +4351,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="1"/>
         <v>('67','hanoi_real','3','The Tower of Hanoi','Reproduce the tower on the right side','Mouse manipulation','The object of the game is to move the entire stack to another peg, obeying the following rules:
@@ -6114,7 +6318,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="str">
         <f t="shared" si="2"/>
         <v>('145','submarine','5','Pilot a submarine','Pilot a submarine using air tanks and dive rudders','Physics basics','Learn how a submarine works'),</v>
@@ -6141,7 +6345,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="str">
         <f t="shared" si="2"/>
         <v>('146','sudoku','4','Sudoku, place unique symbols in a square.','Symbols must be unique in a row, in a column, and (if defined) each region.','Completing the puzzle requires patience and logical ability','The aim of the puzzle is to enter a symbol or numeral from 1 through 9 in each cell of a grid, most frequently a 9x9 grid made up of 3x3 subgrids (called 'regions'), starting with various symbols or numerals given in some cells (the 'givens'). Each row, column and region must contain only one instance of each symbol or numeral (Source &amp;lt;http://en.wikipedia.org/wiki/Sudoku&amp;gt;).'),</v>
@@ -6168,7 +6372,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
         <f t="shared" si="2"/>
         <v>('147','superbrain','2','Super Brain','Tux has hidden several items. Find them again in the correct order','','Tux has hidden several items. Find them again in the correct order'),</v>
@@ -6192,7 +6396,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A148" t="str">
         <f t="shared" si="2"/>
         <v>('148','tangram','1','The tangram puzzle game','The objective is to form a given shape with seven pieces','Mouse-manipulation','From Wikipedia, the free encyclopedia. Tangram (Chinese: literally "seven boards of cunning") is a Chinese puzzle. While the tangram is often said to be ancient, its existence has only been verified as far back as 1800. It consists of 7 pieces, called tans, which fit together to form a square; taking the square as the unit:
@@ -6225,7 +6429,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f t="shared" si="2"/>
         <v>('149','target','2','Practice addition with a target game','Hit the target and count your points','Can move the mouse, can read numbers and count up to 15 for the first level','Throw darts at a target and count your score.'),</v>
@@ -6252,7 +6456,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f t="shared" si="2"/>
         <v>('150','traffic','2','A sliding-block puzzle game','Remove the red car from the parking lot through the gate on the right','','Remove the red car from the parking lot through the gate on the right'),</v>
@@ -6276,7 +6480,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f t="shared" si="2"/>
         <v>('151','watercycle','3','Learn about the water cycle','Tux has come back from a long fishing party on his boat. Bring the water system back up so he can take a shower.','','Learn the water cycle'),</v>
@@ -6300,7 +6504,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f t="shared" si="2"/>
         <v>('152','wordprocessor','2','Your word processor','A simple word processor to enter and save any text','The children can type their own text or copy one given by the teacher.','Learn how to enter text in a wordprocessor. This wordprocessor is special in that it enforces the use of styles. This way, the children will understand their benefit when moving to more feature full wordprocessor like OpenOffice.org.'),</v>
@@ -6327,7 +6531,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
         <f t="shared" si="2"/>
         <v>('153','wordsgame','2','Falling Words','Type the falling words before they reach the ground','Keyboard manipulation','Keyboard training'),</v>
@@ -6352,6 +6556,384 @@
       </c>
       <c r="H153" t="s">
         <v>552</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" t="str">
+        <f t="shared" ref="A156:A168" si="3">CONCATENATE("('", B156,"','",C156,"','",D156,"','",E156,"','",F156,"','",G156,"','",H156,"'),")</f>
+        <v>('154','color_mix','4','Mixing color of paint','To understand color mixing.','','Mix the primary colors to match to the given color'),</v>
+      </c>
+      <c r="B156">
+        <v>154</v>
+      </c>
+      <c r="C156" t="s">
+        <v>553</v>
+      </c>
+      <c r="D156">
+        <v>4</v>
+      </c>
+      <c r="E156" t="s">
+        <v>555</v>
+      </c>
+      <c r="F156" t="s">
+        <v>556</v>
+      </c>
+      <c r="H156" t="s">
+        <v>557</v>
+      </c>
+      <c r="I156" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" t="str">
+        <f t="shared" si="3"/>
+        <v>('155','color_mix_light','1','Mixing colors of light','Understanding mixing of colors of light.','','Mix the primary colors to match to the given color.'),</v>
+      </c>
+      <c r="B157">
+        <v>155</v>
+      </c>
+      <c r="C157" t="s">
+        <v>558</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+      <c r="E157" t="s">
+        <v>560</v>
+      </c>
+      <c r="F157" t="s">
+        <v>561</v>
+      </c>
+      <c r="H157" t="s">
+        <v>562</v>
+      </c>
+      <c r="I157" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" t="str">
+        <f t="shared" si="3"/>
+        <v>('156','explore_farm_animals','2','Explore Farm Animals','Learn about farm animals, what sounds they make, and interesting facts.','','Learn to associate animal sounds with the animal name and what the animal looks like.'),</v>
+      </c>
+      <c r="B158">
+        <v>156</v>
+      </c>
+      <c r="C158" t="s">
+        <v>563</v>
+      </c>
+      <c r="D158">
+        <v>2</v>
+      </c>
+      <c r="E158" t="s">
+        <v>565</v>
+      </c>
+      <c r="F158" t="s">
+        <v>566</v>
+      </c>
+      <c r="H158" t="s">
+        <v>567</v>
+      </c>
+      <c r="I158" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" t="str">
+        <f t="shared" si="3"/>
+        <v>('157','explore_world_animals','4','Explore World Animals','Learn about world animals, interesting facts and their location on a map.','',''),</v>
+      </c>
+      <c r="B159">
+        <v>157</v>
+      </c>
+      <c r="C159" t="s">
+        <v>568</v>
+      </c>
+      <c r="D159">
+        <v>4</v>
+      </c>
+      <c r="E159" t="s">
+        <v>570</v>
+      </c>
+      <c r="F159" t="s">
+        <v>571</v>
+      </c>
+      <c r="I159" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" t="str">
+        <f t="shared" si="3"/>
+        <v>('158','explore_world_music','4','Explore World Music','Learn about the music of the world.','','Develop a better understanding of the variety of music present in the world'),</v>
+      </c>
+      <c r="B160">
+        <v>158</v>
+      </c>
+      <c r="C160" t="s">
+        <v>572</v>
+      </c>
+      <c r="D160">
+        <v>4</v>
+      </c>
+      <c r="E160" t="s">
+        <v>574</v>
+      </c>
+      <c r="F160" t="s">
+        <v>575</v>
+      </c>
+      <c r="H160" t="s">
+        <v>576</v>
+      </c>
+      <c r="I160" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A161" t="str">
+        <f t="shared" si="3"/>
+        <v>('159','intro_gravity','4','Intro gravity','Introduction to the concept of gravity','','Maintain the spaceship in the middle without crashing into the planets or the asteroids'),</v>
+      </c>
+      <c r="B161">
+        <v>159</v>
+      </c>
+      <c r="C161" t="s">
+        <v>577</v>
+      </c>
+      <c r="D161">
+        <v>4</v>
+      </c>
+      <c r="E161" t="s">
+        <v>579</v>
+      </c>
+      <c r="F161" t="s">
+        <v>580</v>
+      </c>
+      <c r="H161" t="s">
+        <v>581</v>
+      </c>
+      <c r="I161" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A162" t="str">
+        <f t="shared" si="3"/>
+        <v>('160','land_safe','4','Land Safe','Understanding acceleration due to gravity.','','Pilot the spaceship towards the green landing area.'),</v>
+      </c>
+      <c r="B162">
+        <v>160</v>
+      </c>
+      <c r="C162" t="s">
+        <v>582</v>
+      </c>
+      <c r="D162">
+        <v>4</v>
+      </c>
+      <c r="E162" t="s">
+        <v>584</v>
+      </c>
+      <c r="F162" t="s">
+        <v>585</v>
+      </c>
+      <c r="H162" t="s">
+        <v>586</v>
+      </c>
+      <c r="I162" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A163" t="str">
+        <f t="shared" si="3"/>
+        <v>('161','mining','1','Mining for gold','Use the mousewheel to approach the rockwall an look for gold nuggets.','You should be familiar with moving the mouse and clicking.','Learn to use the mousewheel to zoom in and out.'),</v>
+      </c>
+      <c r="B163">
+        <v>161</v>
+      </c>
+      <c r="C163" t="s">
+        <v>587</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="E163" t="s">
+        <v>589</v>
+      </c>
+      <c r="F163" t="s">
+        <v>590</v>
+      </c>
+      <c r="G163" t="s">
+        <v>591</v>
+      </c>
+      <c r="H163" t="s">
+        <v>592</v>
+      </c>
+      <c r="I163" t="s">
+        <v>588</v>
+      </c>
+      <c r="Q163" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A164" t="str">
+        <f t="shared" si="3"/>
+        <v>('162','note_names','4','Name that Note!','Learn the names of the notes, in bass and treble clef, with the help of sounds and colors','None','To develop a good understanding of note position and naming convention. To prepare for the piano player and composition activity'),</v>
+      </c>
+      <c r="B164">
+        <v>162</v>
+      </c>
+      <c r="C164" t="s">
+        <v>593</v>
+      </c>
+      <c r="D164">
+        <v>4</v>
+      </c>
+      <c r="E164" t="s">
+        <v>595</v>
+      </c>
+      <c r="F164" t="s">
+        <v>596</v>
+      </c>
+      <c r="G164" t="s">
+        <v>276</v>
+      </c>
+      <c r="H164" t="s">
+        <v>597</v>
+      </c>
+      <c r="I164" t="s">
+        <v>594</v>
+      </c>
+      <c r="Q164" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A165" t="str">
+        <f t="shared" si="3"/>
+        <v>('163','piano_composition','4','Piano Composition','An activity to learn how the piano keyboard works, how notes are written on a musical staff and explore music composition by loading and saving your work.','Familiarity with note naming conventions, note-names activity useful to learn this notation.','Develop an understanding of music composition, and increase interest in making music with a piano keyboard. This activity covers many fundamental aspects of music, but there is much more to explore about music composition. If you enjoy this activity but want a more advanced tool, try downloading MuseScore (http://musescore.org/en/download), an open source music notation tool.'),</v>
+      </c>
+      <c r="B165">
+        <v>163</v>
+      </c>
+      <c r="C165" t="s">
+        <v>598</v>
+      </c>
+      <c r="D165">
+        <v>4</v>
+      </c>
+      <c r="E165" t="s">
+        <v>600</v>
+      </c>
+      <c r="F165" t="s">
+        <v>601</v>
+      </c>
+      <c r="G165" t="s">
+        <v>602</v>
+      </c>
+      <c r="H165" t="s">
+        <v>603</v>
+      </c>
+      <c r="I165" t="s">
+        <v>599</v>
+      </c>
+      <c r="Q165" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A166" t="str">
+        <f t="shared" si="3"/>
+        <v>('164','place_your_satellite','4','Place your satellite','Understanding effect of mass and distance on orbital velocity.','','Make sure the satellite does not crash or fly away'),</v>
+      </c>
+      <c r="B166">
+        <v>164</v>
+      </c>
+      <c r="C166" t="s">
+        <v>604</v>
+      </c>
+      <c r="D166">
+        <v>4</v>
+      </c>
+      <c r="E166" t="s">
+        <v>606</v>
+      </c>
+      <c r="F166" t="s">
+        <v>607</v>
+      </c>
+      <c r="H166" t="s">
+        <v>608</v>
+      </c>
+      <c r="I166" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A167" t="str">
+        <f t="shared" si="3"/>
+        <v>('165','play_piano','2','Play Piano!','Learn to play melodies on the piano keyboard!','Knowledge of musical notation and musical staff. Play the activity named 'Piano Composition' first.','Understand how the piano keyboard can play music as written on the musical staff.'),</v>
+      </c>
+      <c r="B167">
+        <v>165</v>
+      </c>
+      <c r="C167" t="s">
+        <v>609</v>
+      </c>
+      <c r="D167">
+        <v>2</v>
+      </c>
+      <c r="E167" t="s">
+        <v>611</v>
+      </c>
+      <c r="F167" t="s">
+        <v>612</v>
+      </c>
+      <c r="G167" t="s">
+        <v>613</v>
+      </c>
+      <c r="H167" t="s">
+        <v>614</v>
+      </c>
+      <c r="I167" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q167" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A168" t="str">
+        <f t="shared" si="3"/>
+        <v>('166','play_rhythm','3','Play Rhythm','Learn to listen to, read, and play musical rhythms.','Simple understanding of musical rhythm and beat.','Learn to beat rhythms precisely and accurately based on what you see and hear.'),</v>
+      </c>
+      <c r="B168">
+        <v>166</v>
+      </c>
+      <c r="C168" t="s">
+        <v>615</v>
+      </c>
+      <c r="D168">
+        <v>3</v>
+      </c>
+      <c r="E168" t="s">
+        <v>617</v>
+      </c>
+      <c r="F168" t="s">
+        <v>618</v>
+      </c>
+      <c r="G168" t="s">
+        <v>619</v>
+      </c>
+      <c r="H168" t="s">
+        <v>620</v>
+      </c>
+      <c r="I168" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q168" t="s">
+        <v>619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>